<commit_message>
added boolean to print edge plot
</commit_message>
<xml_diff>
--- a/computational_study/comp_study_summary.xlsx
+++ b/computational_study/comp_study_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tordhaflan/Dropbox/NTNU/Master/master-thesis/computational study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tordhaflan/Dropbox/NTNU/Master/master-thesis/computational_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7426BC5-24C8-D244-8B6D-1A247AE3D812}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D56D2A-F11C-CF40-85B2-F780DF73EC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,28 +32,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -80,10 +58,10 @@
     <t>Time horizont</t>
   </si>
   <si>
-    <t>Scooters</t>
+    <t>Scooters/zone</t>
   </si>
   <si>
-    <t>Scooters/zone</t>
+    <t>Scooters</t>
   </si>
 </sst>
 </file>
@@ -91,8 +69,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\V\ \=\ #,##0"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="\V\ \=\ #,##0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -145,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -261,12 +239,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -276,28 +267,32 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -308,27 +303,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -649,10 +633,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2751,7 +2735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486AFFF7-E276-0D49-92B4-8CCBAB0B41C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="126" workbookViewId="0">
@@ -2760,17 +2744,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" style="5" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -2833,21 +2817,20 @@
       <c r="G2" s="2">
         <v>0.25456000000000001</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="24">
-        <v>1</v>
-      </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="24">
-        <v>2</v>
-      </c>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="24">
-        <v>3</v>
-      </c>
-      <c r="R2" s="25"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="27">
+        <v>1</v>
+      </c>
+      <c r="N2" s="26"/>
+      <c r="O2" s="27">
+        <v>2</v>
+      </c>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27">
+        <v>3</v>
+      </c>
+      <c r="R2" s="26"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -2871,31 +2854,31 @@
       <c r="G3" s="2">
         <v>0.19075</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2924,37 +2907,37 @@
       <c r="I4" s="4">
         <v>20</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="24">
         <v>20</v>
       </c>
       <c r="K4" s="18">
         <v>2</v>
       </c>
-      <c r="L4" s="12">
-        <f>K4*4</f>
+      <c r="L4" s="9">
+        <f t="shared" ref="L4:L33" si="0">K4*4</f>
         <v>8</v>
       </c>
-      <c r="M4" s="8" cm="1">
+      <c r="M4" s="21">
         <f t="array" ref="M4">INDEX($F$2:$G$91,MATCH($K4&amp;M$1&amp;$I4,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>2.1420000000000002E-2</v>
       </c>
-      <c r="N4" s="9" cm="1">
+      <c r="N4" s="7">
         <f t="array" ref="N4">INDEX($F$2:$G$91,MATCH($K4&amp;N$1&amp;$I4,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O4" s="8" cm="1">
+      <c r="O4" s="21">
         <f t="array" ref="O4">INDEX($F$2:$G$91,MATCH($K4&amp;O$1&amp;$I4,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="P4" s="9" cm="1">
+      <c r="P4" s="7">
         <f t="array" ref="P4">INDEX($F$2:$G$91,MATCH($K4&amp;P$1&amp;$I4,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="8" cm="1">
+      <c r="Q4" s="21">
         <f t="array" ref="Q4">INDEX($F$2:$G$91,MATCH($K4&amp;Q$1&amp;$I4,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>1.2789999999999999E-2</v>
       </c>
-      <c r="R4" s="9" cm="1">
+      <c r="R4" s="7">
         <f t="array" ref="R4">INDEX($F$2:$G$91,MATCH($K4&amp;R$1&amp;$I4,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -2984,35 +2967,35 @@
       <c r="I5" s="4">
         <v>20</v>
       </c>
-      <c r="J5" s="27"/>
+      <c r="J5" s="25"/>
       <c r="K5" s="19">
         <v>3</v>
       </c>
-      <c r="L5" s="13">
-        <f t="shared" ref="L5:L33" si="0">K5*4</f>
+      <c r="L5" s="10">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M5" s="6" cm="1">
+      <c r="M5" s="22">
         <f t="array" ref="M5">INDEX($F$2:$G$91,MATCH($K5&amp;M$1&amp;$I5,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>0.27124999999999999</v>
       </c>
-      <c r="N5" s="7" cm="1">
+      <c r="N5" s="6">
         <f t="array" ref="N5">INDEX($F$2:$G$91,MATCH($K5&amp;N$1&amp;$I5,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O5" s="6" cm="1">
+      <c r="O5" s="22">
         <f t="array" ref="O5">INDEX($F$2:$G$91,MATCH($K5&amp;O$1&amp;$I5,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>0.64436000000000004</v>
       </c>
-      <c r="P5" s="7" cm="1">
+      <c r="P5" s="6">
         <f t="array" ref="P5">INDEX($F$2:$G$91,MATCH($K5&amp;P$1&amp;$I5,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="6" cm="1">
+      <c r="Q5" s="22">
         <f t="array" ref="Q5">INDEX($F$2:$G$91,MATCH($K5&amp;Q$1&amp;$I5,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>3.6753499999999999</v>
       </c>
-      <c r="R5" s="7" cm="1">
+      <c r="R5" s="6">
         <f t="array" ref="R5">INDEX($F$2:$G$91,MATCH($K5&amp;R$1&amp;$I5,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3042,35 +3025,35 @@
       <c r="I6" s="4">
         <v>20</v>
       </c>
-      <c r="J6" s="27"/>
+      <c r="J6" s="25"/>
       <c r="K6" s="19">
         <v>4</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M6" s="6" cm="1">
+      <c r="M6" s="22">
         <f t="array" ref="M6">INDEX($F$2:$G$91,MATCH($K6&amp;M$1&amp;$I6,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>0.44366</v>
       </c>
-      <c r="N6" s="7" cm="1">
+      <c r="N6" s="6">
         <f t="array" ref="N6">INDEX($F$2:$G$91,MATCH($K6&amp;N$1&amp;$I6,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O6" s="6" cm="1">
+      <c r="O6" s="22">
         <f t="array" ref="O6">INDEX($F$2:$G$91,MATCH($K6&amp;O$1&amp;$I6,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>1.4904299999999999</v>
       </c>
-      <c r="P6" s="7" cm="1">
+      <c r="P6" s="6">
         <f t="array" ref="P6">INDEX($F$2:$G$91,MATCH($K6&amp;P$1&amp;$I6,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="6" cm="1">
+      <c r="Q6" s="22">
         <f t="array" ref="Q6">INDEX($F$2:$G$91,MATCH($K6&amp;Q$1&amp;$I6,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.01312999999999</v>
       </c>
-      <c r="R6" s="7" cm="1">
+      <c r="R6" s="6">
         <f t="array" ref="R6">INDEX($F$2:$G$91,MATCH($K6&amp;R$1&amp;$I6,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>8.0400000000000003E-3</v>
       </c>
@@ -3100,35 +3083,35 @@
       <c r="I7" s="4">
         <v>20</v>
       </c>
-      <c r="J7" s="27"/>
+      <c r="J7" s="25"/>
       <c r="K7" s="19">
         <v>5</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="M7" s="6" cm="1">
+      <c r="M7" s="22">
         <f t="array" ref="M7">INDEX($F$2:$G$91,MATCH($K7&amp;M$1&amp;$I7,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>0.71687000000000001</v>
       </c>
-      <c r="N7" s="7" cm="1">
+      <c r="N7" s="6">
         <f t="array" ref="N7">INDEX($F$2:$G$91,MATCH($K7&amp;N$1&amp;$I7,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O7" s="6" cm="1">
+      <c r="O7" s="22">
         <f t="array" ref="O7">INDEX($F$2:$G$91,MATCH($K7&amp;O$1&amp;$I7,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>1.69689</v>
       </c>
-      <c r="P7" s="7" cm="1">
+      <c r="P7" s="6">
         <f t="array" ref="P7">INDEX($F$2:$G$91,MATCH($K7&amp;P$1&amp;$I7,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="6" cm="1">
+      <c r="Q7" s="22">
         <f t="array" ref="Q7">INDEX($F$2:$G$91,MATCH($K7&amp;Q$1&amp;$I7,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>77.459050000000005</v>
       </c>
-      <c r="R7" s="7" cm="1">
+      <c r="R7" s="6">
         <f t="array" ref="R7">INDEX($F$2:$G$91,MATCH($K7&amp;R$1&amp;$I7,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3158,35 +3141,35 @@
       <c r="I8" s="4">
         <v>20</v>
       </c>
-      <c r="J8" s="27"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="19">
         <v>6</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="M8" s="6" cm="1">
+      <c r="M8" s="22">
         <f t="array" ref="M8">INDEX($F$2:$G$91,MATCH($K8&amp;M$1&amp;$I8,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>15.661199999999999</v>
       </c>
-      <c r="N8" s="7" cm="1">
+      <c r="N8" s="6">
         <f t="array" ref="N8">INDEX($F$2:$G$91,MATCH($K8&amp;N$1&amp;$I8,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O8" s="6" cm="1">
+      <c r="O8" s="22">
         <f t="array" ref="O8">INDEX($F$2:$G$91,MATCH($K8&amp;O$1&amp;$I8,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>21.926870000000001</v>
       </c>
-      <c r="P8" s="7" cm="1">
+      <c r="P8" s="6">
         <f t="array" ref="P8">INDEX($F$2:$G$91,MATCH($K8&amp;P$1&amp;$I8,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="6" cm="1">
+      <c r="Q8" s="22">
         <f t="array" ref="Q8">INDEX($F$2:$G$91,MATCH($K8&amp;Q$1&amp;$I8,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.01533000000001</v>
       </c>
-      <c r="R8" s="7" cm="1">
+      <c r="R8" s="6">
         <f t="array" ref="R8">INDEX($F$2:$G$91,MATCH($K8&amp;R$1&amp;$I8,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0.19075</v>
       </c>
@@ -3216,35 +3199,35 @@
       <c r="I9" s="4">
         <v>20</v>
       </c>
-      <c r="J9" s="28"/>
+      <c r="J9" s="26"/>
       <c r="K9" s="20">
         <v>7</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="11">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M9" s="10" cm="1">
+      <c r="M9" s="23">
         <f t="array" ref="M9">INDEX($F$2:$G$91,MATCH($K9&amp;M$1&amp;$I9,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01441999999997</v>
       </c>
-      <c r="N9" s="11" cm="1">
+      <c r="N9" s="8">
         <f t="array" ref="N9">INDEX($F$2:$G$91,MATCH($K9&amp;N$1&amp;$I9,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.17274</v>
       </c>
-      <c r="O9" s="10" cm="1">
+      <c r="O9" s="23">
         <f t="array" ref="O9">INDEX($F$2:$G$91,MATCH($K9&amp;O$1&amp;$I9,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>297.22269</v>
       </c>
-      <c r="P9" s="11" cm="1">
+      <c r="P9" s="8">
         <f t="array" ref="P9">INDEX($F$2:$G$91,MATCH($K9&amp;P$1&amp;$I9,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="10" cm="1">
+      <c r="Q9" s="23">
         <f t="array" ref="Q9">INDEX($F$2:$G$91,MATCH($K9&amp;Q$1&amp;$I9,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.03390000000002</v>
       </c>
-      <c r="R9" s="11" cm="1">
+      <c r="R9" s="8">
         <f t="array" ref="R9">INDEX($F$2:$G$91,MATCH($K9&amp;R$1&amp;$I9,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0.25456000000000001</v>
       </c>
@@ -3274,37 +3257,37 @@
       <c r="I10" s="4">
         <v>30</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="24">
         <v>30</v>
       </c>
       <c r="K10" s="18">
         <v>2</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M10" s="8" cm="1">
+      <c r="M10" s="21">
         <f t="array" ref="M10">INDEX($F$2:$G$91,MATCH($K10&amp;M$1&amp;$I10,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>2.8989999999999998E-2</v>
       </c>
-      <c r="N10" s="9" cm="1">
+      <c r="N10" s="7">
         <f t="array" ref="N10">INDEX($F$2:$G$91,MATCH($K10&amp;N$1&amp;$I10,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O10" s="8" cm="1">
+      <c r="O10" s="21">
         <f t="array" ref="O10">INDEX($F$2:$G$91,MATCH($K10&amp;O$1&amp;$I10,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>1.503E-2</v>
       </c>
-      <c r="P10" s="9" cm="1">
+      <c r="P10" s="7">
         <f t="array" ref="P10">INDEX($F$2:$G$91,MATCH($K10&amp;P$1&amp;$I10,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="8" cm="1">
+      <c r="Q10" s="21">
         <f t="array" ref="Q10">INDEX($F$2:$G$91,MATCH($K10&amp;Q$1&amp;$I10,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>1.401E-2</v>
       </c>
-      <c r="R10" s="9" cm="1">
+      <c r="R10" s="7">
         <f t="array" ref="R10">INDEX($F$2:$G$91,MATCH($K10&amp;R$1&amp;$I10,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3334,35 +3317,35 @@
       <c r="I11" s="4">
         <v>30</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="19">
         <v>3</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M11" s="6" cm="1">
+      <c r="M11" s="22">
         <f t="array" ref="M11">INDEX($F$2:$G$91,MATCH($K11&amp;M$1&amp;$I11,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>0.20974000000000001</v>
       </c>
-      <c r="N11" s="7" cm="1">
+      <c r="N11" s="6">
         <f t="array" ref="N11">INDEX($F$2:$G$91,MATCH($K11&amp;N$1&amp;$I11,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O11" s="6" cm="1">
+      <c r="O11" s="22">
         <f t="array" ref="O11">INDEX($F$2:$G$91,MATCH($K11&amp;O$1&amp;$I11,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>1.5492699999999999</v>
       </c>
-      <c r="P11" s="7" cm="1">
+      <c r="P11" s="6">
         <f t="array" ref="P11">INDEX($F$2:$G$91,MATCH($K11&amp;P$1&amp;$I11,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="6" cm="1">
+      <c r="Q11" s="22">
         <f t="array" ref="Q11">INDEX($F$2:$G$91,MATCH($K11&amp;Q$1&amp;$I11,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>0.48616999999999999</v>
       </c>
-      <c r="R11" s="7" cm="1">
+      <c r="R11" s="6">
         <f t="array" ref="R11">INDEX($F$2:$G$91,MATCH($K11&amp;R$1&amp;$I11,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3392,35 +3375,35 @@
       <c r="I12" s="4">
         <v>30</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="25"/>
       <c r="K12" s="19">
         <v>4</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M12" s="6" cm="1">
+      <c r="M12" s="22">
         <f t="array" ref="M12">INDEX($F$2:$G$91,MATCH($K12&amp;M$1&amp;$I12,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>1.0864799999999999</v>
       </c>
-      <c r="N12" s="7" cm="1">
+      <c r="N12" s="6">
         <f t="array" ref="N12">INDEX($F$2:$G$91,MATCH($K12&amp;N$1&amp;$I12,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O12" s="6" cm="1">
+      <c r="O12" s="22">
         <f t="array" ref="O12">INDEX($F$2:$G$91,MATCH($K12&amp;O$1&amp;$I12,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>6.4286899999999996</v>
       </c>
-      <c r="P12" s="7" cm="1">
+      <c r="P12" s="6">
         <f t="array" ref="P12">INDEX($F$2:$G$91,MATCH($K12&amp;P$1&amp;$I12,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="6" cm="1">
+      <c r="Q12" s="22">
         <f t="array" ref="Q12">INDEX($F$2:$G$91,MATCH($K12&amp;Q$1&amp;$I12,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>2.9802399999999998</v>
       </c>
-      <c r="R12" s="7" cm="1">
+      <c r="R12" s="6">
         <f t="array" ref="R12">INDEX($F$2:$G$91,MATCH($K12&amp;R$1&amp;$I12,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3450,35 +3433,35 @@
       <c r="I13" s="4">
         <v>30</v>
       </c>
-      <c r="J13" s="27"/>
+      <c r="J13" s="25"/>
       <c r="K13" s="19">
         <v>5</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="M13" s="6" cm="1">
+      <c r="M13" s="22">
         <f t="array" ref="M13">INDEX($F$2:$G$91,MATCH($K13&amp;M$1&amp;$I13,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00916000000001</v>
       </c>
-      <c r="N13" s="7" cm="1">
+      <c r="N13" s="6">
         <f t="array" ref="N13">INDEX($F$2:$G$91,MATCH($K13&amp;N$1&amp;$I13,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>6.676E-2</v>
       </c>
-      <c r="O13" s="6" cm="1">
+      <c r="O13" s="22">
         <f t="array" ref="O13">INDEX($F$2:$G$91,MATCH($K13&amp;O$1&amp;$I13,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>132.98533</v>
       </c>
-      <c r="P13" s="7" cm="1">
+      <c r="P13" s="6">
         <f t="array" ref="P13">INDEX($F$2:$G$91,MATCH($K13&amp;P$1&amp;$I13,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="6" cm="1">
+      <c r="Q13" s="22">
         <f t="array" ref="Q13">INDEX($F$2:$G$91,MATCH($K13&amp;Q$1&amp;$I13,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.01375999999999</v>
       </c>
-      <c r="R13" s="7" cm="1">
+      <c r="R13" s="6">
         <f t="array" ref="R13">INDEX($F$2:$G$91,MATCH($K13&amp;R$1&amp;$I13,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>6.0600000000000003E-3</v>
       </c>
@@ -3508,35 +3491,35 @@
       <c r="I14" s="4">
         <v>30</v>
       </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="19">
         <v>6</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="M14" s="6" cm="1">
+      <c r="M14" s="22">
         <f t="array" ref="M14">INDEX($F$2:$G$91,MATCH($K14&amp;M$1&amp;$I14,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00941999999998</v>
       </c>
-      <c r="N14" s="7" cm="1">
+      <c r="N14" s="6">
         <f t="array" ref="N14">INDEX($F$2:$G$91,MATCH($K14&amp;N$1&amp;$I14,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.37905</v>
       </c>
-      <c r="O14" s="6" cm="1">
+      <c r="O14" s="22">
         <f t="array" ref="O14">INDEX($F$2:$G$91,MATCH($K14&amp;O$1&amp;$I14,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01821999999999</v>
       </c>
-      <c r="P14" s="7" cm="1">
+      <c r="P14" s="6">
         <f t="array" ref="P14">INDEX($F$2:$G$91,MATCH($K14&amp;P$1&amp;$I14,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.18487000000000001</v>
       </c>
-      <c r="Q14" s="6" cm="1">
+      <c r="Q14" s="22">
         <f t="array" ref="Q14">INDEX($F$2:$G$91,MATCH($K14&amp;Q$1&amp;$I14,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.01792999999998</v>
       </c>
-      <c r="R14" s="7" cm="1">
+      <c r="R14" s="6">
         <f t="array" ref="R14">INDEX($F$2:$G$91,MATCH($K14&amp;R$1&amp;$I14,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>2.3050000000000001E-2</v>
       </c>
@@ -3566,35 +3549,35 @@
       <c r="I15" s="4">
         <v>30</v>
       </c>
-      <c r="J15" s="28"/>
+      <c r="J15" s="26"/>
       <c r="K15" s="20">
         <v>7</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="11">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M15" s="10" cm="1">
+      <c r="M15" s="23">
         <f t="array" ref="M15">INDEX($F$2:$G$91,MATCH($K15&amp;M$1&amp;$I15,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01542000000001</v>
       </c>
-      <c r="N15" s="11" cm="1">
+      <c r="N15" s="8">
         <f t="array" ref="N15">INDEX($F$2:$G$91,MATCH($K15&amp;N$1&amp;$I15,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.56025999999999998</v>
       </c>
-      <c r="O15" s="10" cm="1">
+      <c r="O15" s="23">
         <f t="array" ref="O15">INDEX($F$2:$G$91,MATCH($K15&amp;O$1&amp;$I15,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01927000000001</v>
       </c>
-      <c r="P15" s="11" cm="1">
+      <c r="P15" s="8">
         <f t="array" ref="P15">INDEX($F$2:$G$91,MATCH($K15&amp;P$1&amp;$I15,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.37308999999999998</v>
       </c>
-      <c r="Q15" s="10" cm="1">
+      <c r="Q15" s="23">
         <f t="array" ref="Q15">INDEX($F$2:$G$91,MATCH($K15&amp;Q$1&amp;$I15,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.02366000000001</v>
       </c>
-      <c r="R15" s="11" cm="1">
+      <c r="R15" s="8">
         <f t="array" ref="R15">INDEX($F$2:$G$91,MATCH($K15&amp;R$1&amp;$I15,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>7.9079999999999998E-2</v>
       </c>
@@ -3624,37 +3607,37 @@
       <c r="I16" s="4">
         <v>40</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="24">
         <v>40</v>
       </c>
       <c r="K16" s="18">
         <v>2</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M16" s="8" cm="1">
+      <c r="M16" s="21">
         <f t="array" ref="M16">INDEX($F$2:$G$91,MATCH($K16&amp;M$1&amp;$I16,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>4.1399999999999996E-3</v>
       </c>
-      <c r="N16" s="9" cm="1">
+      <c r="N16" s="7">
         <f t="array" ref="N16">INDEX($F$2:$G$91,MATCH($K16&amp;N$1&amp;$I16,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O16" s="8" cm="1">
+      <c r="O16" s="21">
         <f t="array" ref="O16">INDEX($F$2:$G$91,MATCH($K16&amp;O$1&amp;$I16,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>7.43E-3</v>
       </c>
-      <c r="P16" s="9" cm="1">
+      <c r="P16" s="7">
         <f t="array" ref="P16">INDEX($F$2:$G$91,MATCH($K16&amp;P$1&amp;$I16,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="8" cm="1">
+      <c r="Q16" s="21">
         <f t="array" ref="Q16">INDEX($F$2:$G$91,MATCH($K16&amp;Q$1&amp;$I16,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>1.404E-2</v>
       </c>
-      <c r="R16" s="9" cm="1">
+      <c r="R16" s="7">
         <f t="array" ref="R16">INDEX($F$2:$G$91,MATCH($K16&amp;R$1&amp;$I16,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3684,35 +3667,35 @@
       <c r="I17" s="4">
         <v>40</v>
       </c>
-      <c r="J17" s="27"/>
+      <c r="J17" s="25"/>
       <c r="K17" s="19">
         <v>3</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M17" s="6" cm="1">
+      <c r="M17" s="22">
         <f t="array" ref="M17">INDEX($F$2:$G$91,MATCH($K17&amp;M$1&amp;$I17,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>0.2414</v>
       </c>
-      <c r="N17" s="7" cm="1">
+      <c r="N17" s="6">
         <f t="array" ref="N17">INDEX($F$2:$G$91,MATCH($K17&amp;N$1&amp;$I17,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O17" s="6" cm="1">
+      <c r="O17" s="22">
         <f t="array" ref="O17">INDEX($F$2:$G$91,MATCH($K17&amp;O$1&amp;$I17,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>9.8320000000000005E-2</v>
       </c>
-      <c r="P17" s="7" cm="1">
+      <c r="P17" s="6">
         <f t="array" ref="P17">INDEX($F$2:$G$91,MATCH($K17&amp;P$1&amp;$I17,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="6" cm="1">
+      <c r="Q17" s="22">
         <f t="array" ref="Q17">INDEX($F$2:$G$91,MATCH($K17&amp;Q$1&amp;$I17,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>0.27685999999999999</v>
       </c>
-      <c r="R17" s="7" cm="1">
+      <c r="R17" s="6">
         <f t="array" ref="R17">INDEX($F$2:$G$91,MATCH($K17&amp;R$1&amp;$I17,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3742,35 +3725,35 @@
       <c r="I18" s="4">
         <v>40</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="19">
         <v>4</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M18" s="6" cm="1">
+      <c r="M18" s="22">
         <f t="array" ref="M18">INDEX($F$2:$G$91,MATCH($K18&amp;M$1&amp;$I18,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00767000000002</v>
       </c>
-      <c r="N18" s="7" cm="1">
+      <c r="N18" s="6">
         <f t="array" ref="N18">INDEX($F$2:$G$91,MATCH($K18&amp;N$1&amp;$I18,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>5.5809999999999998E-2</v>
       </c>
-      <c r="O18" s="6" cm="1">
+      <c r="O18" s="22">
         <f t="array" ref="O18">INDEX($F$2:$G$91,MATCH($K18&amp;O$1&amp;$I18,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.07324999999997</v>
       </c>
-      <c r="P18" s="7" cm="1">
+      <c r="P18" s="6">
         <f t="array" ref="P18">INDEX($F$2:$G$91,MATCH($K18&amp;P$1&amp;$I18,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>2.8729999999999999E-2</v>
       </c>
-      <c r="Q18" s="6" cm="1">
+      <c r="Q18" s="22">
         <f t="array" ref="Q18">INDEX($F$2:$G$91,MATCH($K18&amp;Q$1&amp;$I18,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>0.29807</v>
       </c>
-      <c r="R18" s="7" cm="1">
+      <c r="R18" s="6">
         <f t="array" ref="R18">INDEX($F$2:$G$91,MATCH($K18&amp;R$1&amp;$I18,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -3800,35 +3783,35 @@
       <c r="I19" s="4">
         <v>40</v>
       </c>
-      <c r="J19" s="27"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="19">
         <v>5</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="M19" s="6" cm="1">
+      <c r="M19" s="22">
         <f t="array" ref="M19">INDEX($F$2:$G$91,MATCH($K19&amp;M$1&amp;$I19,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00761999999997</v>
       </c>
-      <c r="N19" s="7" cm="1">
+      <c r="N19" s="6">
         <f t="array" ref="N19">INDEX($F$2:$G$91,MATCH($K19&amp;N$1&amp;$I19,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.23433000000000001</v>
       </c>
-      <c r="O19" s="6" cm="1">
+      <c r="O19" s="22">
         <f t="array" ref="O19">INDEX($F$2:$G$91,MATCH($K19&amp;O$1&amp;$I19,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01398</v>
       </c>
-      <c r="P19" s="7" cm="1">
+      <c r="P19" s="6">
         <f t="array" ref="P19">INDEX($F$2:$G$91,MATCH($K19&amp;P$1&amp;$I19,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.12731000000000001</v>
       </c>
-      <c r="Q19" s="6" cm="1">
+      <c r="Q19" s="22">
         <f t="array" ref="Q19">INDEX($F$2:$G$91,MATCH($K19&amp;Q$1&amp;$I19,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.04050999999998</v>
       </c>
-      <c r="R19" s="7" cm="1">
+      <c r="R19" s="6">
         <f t="array" ref="R19">INDEX($F$2:$G$91,MATCH($K19&amp;R$1&amp;$I19,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>1.01E-3</v>
       </c>
@@ -3858,35 +3841,35 @@
       <c r="I20" s="4">
         <v>40</v>
       </c>
-      <c r="J20" s="27"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="19">
         <v>6</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="M20" s="6" cm="1">
+      <c r="M20" s="22">
         <f t="array" ref="M20">INDEX($F$2:$G$91,MATCH($K20&amp;M$1&amp;$I20,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00486999999998</v>
       </c>
-      <c r="N20" s="7" cm="1">
+      <c r="N20" s="6">
         <f t="array" ref="N20">INDEX($F$2:$G$91,MATCH($K20&amp;N$1&amp;$I20,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.33607999999999999</v>
       </c>
-      <c r="O20" s="6" cm="1">
+      <c r="O20" s="22">
         <f t="array" ref="O20">INDEX($F$2:$G$91,MATCH($K20&amp;O$1&amp;$I20,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01247999999998</v>
       </c>
-      <c r="P20" s="7" cm="1">
+      <c r="P20" s="6">
         <f t="array" ref="P20">INDEX($F$2:$G$91,MATCH($K20&amp;P$1&amp;$I20,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.25947999999999999</v>
       </c>
-      <c r="Q20" s="6" cm="1">
+      <c r="Q20" s="22">
         <f t="array" ref="Q20">INDEX($F$2:$G$91,MATCH($K20&amp;Q$1&amp;$I20,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.02685000000002</v>
       </c>
-      <c r="R20" s="7" cm="1">
+      <c r="R20" s="6">
         <f t="array" ref="R20">INDEX($F$2:$G$91,MATCH($K20&amp;R$1&amp;$I20,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>1.6250000000000001E-2</v>
       </c>
@@ -3916,35 +3899,35 @@
       <c r="I21" s="4">
         <v>40</v>
       </c>
-      <c r="J21" s="28"/>
+      <c r="J21" s="26"/>
       <c r="K21" s="20">
         <v>7</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="11">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M21" s="10" cm="1">
+      <c r="M21" s="23">
         <f t="array" ref="M21">INDEX($F$2:$G$91,MATCH($K21&amp;M$1&amp;$I21,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01961</v>
       </c>
-      <c r="N21" s="11" cm="1">
+      <c r="N21" s="8">
         <f t="array" ref="N21">INDEX($F$2:$G$91,MATCH($K21&amp;N$1&amp;$I21,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.39058999999999999</v>
       </c>
-      <c r="O21" s="10" cm="1">
+      <c r="O21" s="23">
         <f t="array" ref="O21">INDEX($F$2:$G$91,MATCH($K21&amp;O$1&amp;$I21,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01844999999997</v>
       </c>
-      <c r="P21" s="11" cm="1">
+      <c r="P21" s="8">
         <f t="array" ref="P21">INDEX($F$2:$G$91,MATCH($K21&amp;P$1&amp;$I21,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.30647999999999997</v>
       </c>
-      <c r="Q21" s="10" cm="1">
+      <c r="Q21" s="23">
         <f t="array" ref="Q21">INDEX($F$2:$G$91,MATCH($K21&amp;Q$1&amp;$I21,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.03233</v>
       </c>
-      <c r="R21" s="11" cm="1">
+      <c r="R21" s="8">
         <f t="array" ref="R21">INDEX($F$2:$G$91,MATCH($K21&amp;R$1&amp;$I21,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>7.8380000000000005E-2</v>
       </c>
@@ -3974,37 +3957,37 @@
       <c r="I22" s="4">
         <v>50</v>
       </c>
-      <c r="J22" s="26">
+      <c r="J22" s="24">
         <v>50</v>
       </c>
       <c r="K22" s="18">
         <v>2</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M22" s="8" cm="1">
+      <c r="M22" s="21">
         <f t="array" ref="M22">INDEX($F$2:$G$91,MATCH($K22&amp;M$1&amp;$I22,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>3.98E-3</v>
       </c>
-      <c r="N22" s="9" cm="1">
+      <c r="N22" s="7">
         <f t="array" ref="N22">INDEX($F$2:$G$91,MATCH($K22&amp;N$1&amp;$I22,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O22" s="8" cm="1">
+      <c r="O22" s="21">
         <f t="array" ref="O22">INDEX($F$2:$G$91,MATCH($K22&amp;O$1&amp;$I22,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>7.1300000000000001E-3</v>
       </c>
-      <c r="P22" s="9" cm="1">
+      <c r="P22" s="7">
         <f t="array" ref="P22">INDEX($F$2:$G$91,MATCH($K22&amp;P$1&amp;$I22,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="8" cm="1">
+      <c r="Q22" s="21">
         <f t="array" ref="Q22">INDEX($F$2:$G$91,MATCH($K22&amp;Q$1&amp;$I22,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>1.1220000000000001E-2</v>
       </c>
-      <c r="R22" s="9" cm="1">
+      <c r="R22" s="7">
         <f t="array" ref="R22">INDEX($F$2:$G$91,MATCH($K22&amp;R$1&amp;$I22,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -4034,35 +4017,35 @@
       <c r="I23" s="4">
         <v>50</v>
       </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="25"/>
       <c r="K23" s="19">
         <v>3</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L23" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M23" s="6" cm="1">
+      <c r="M23" s="22">
         <f t="array" ref="M23">INDEX($F$2:$G$91,MATCH($K23&amp;M$1&amp;$I23,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>261.56679000000003</v>
       </c>
-      <c r="N23" s="7" cm="1">
+      <c r="N23" s="6">
         <f t="array" ref="N23">INDEX($F$2:$G$91,MATCH($K23&amp;N$1&amp;$I23,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O23" s="6" cm="1">
+      <c r="O23" s="22">
         <f t="array" ref="O23">INDEX($F$2:$G$91,MATCH($K23&amp;O$1&amp;$I23,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>0.29248000000000002</v>
       </c>
-      <c r="P23" s="7" cm="1">
+      <c r="P23" s="6">
         <f t="array" ref="P23">INDEX($F$2:$G$91,MATCH($K23&amp;P$1&amp;$I23,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="6" cm="1">
+      <c r="Q23" s="22">
         <f t="array" ref="Q23">INDEX($F$2:$G$91,MATCH($K23&amp;Q$1&amp;$I23,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>0.17843999999999999</v>
       </c>
-      <c r="R23" s="7" cm="1">
+      <c r="R23" s="6">
         <f t="array" ref="R23">INDEX($F$2:$G$91,MATCH($K23&amp;R$1&amp;$I23,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -4092,35 +4075,35 @@
       <c r="I24" s="4">
         <v>50</v>
       </c>
-      <c r="J24" s="27"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="19">
         <v>4</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M24" s="6" cm="1">
+      <c r="M24" s="22">
         <f t="array" ref="M24">INDEX($F$2:$G$91,MATCH($K24&amp;M$1&amp;$I24,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01483000000002</v>
       </c>
-      <c r="N24" s="7" cm="1">
+      <c r="N24" s="6">
         <f t="array" ref="N24">INDEX($F$2:$G$91,MATCH($K24&amp;N$1&amp;$I24,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.10256</v>
       </c>
-      <c r="O24" s="6" cm="1">
+      <c r="O24" s="22">
         <f t="array" ref="O24">INDEX($F$2:$G$91,MATCH($K24&amp;O$1&amp;$I24,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01096000000001</v>
       </c>
-      <c r="P24" s="7" cm="1">
+      <c r="P24" s="6">
         <f t="array" ref="P24">INDEX($F$2:$G$91,MATCH($K24&amp;P$1&amp;$I24,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>2.8729999999999999E-2</v>
       </c>
-      <c r="Q24" s="6" cm="1">
+      <c r="Q24" s="22">
         <f t="array" ref="Q24">INDEX($F$2:$G$91,MATCH($K24&amp;Q$1&amp;$I24,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>0.34788999999999998</v>
       </c>
-      <c r="R24" s="7" cm="1">
+      <c r="R24" s="6">
         <f t="array" ref="R24">INDEX($F$2:$G$91,MATCH($K24&amp;R$1&amp;$I24,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -4150,35 +4133,35 @@
       <c r="I25" s="4">
         <v>50</v>
       </c>
-      <c r="J25" s="27"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="19">
         <v>5</v>
       </c>
-      <c r="L25" s="13">
+      <c r="L25" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="M25" s="6" cm="1">
+      <c r="M25" s="22">
         <f t="array" ref="M25">INDEX($F$2:$G$91,MATCH($K25&amp;M$1&amp;$I25,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.02159</v>
       </c>
-      <c r="N25" s="7" cm="1">
+      <c r="N25" s="6">
         <f t="array" ref="N25">INDEX($F$2:$G$91,MATCH($K25&amp;N$1&amp;$I25,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.23433000000000001</v>
       </c>
-      <c r="O25" s="6" cm="1">
+      <c r="O25" s="22">
         <f t="array" ref="O25">INDEX($F$2:$G$91,MATCH($K25&amp;O$1&amp;$I25,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.00711999999999</v>
       </c>
-      <c r="P25" s="7" cm="1">
+      <c r="P25" s="6">
         <f t="array" ref="P25">INDEX($F$2:$G$91,MATCH($K25&amp;P$1&amp;$I25,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.12731000000000001</v>
       </c>
-      <c r="Q25" s="6" cm="1">
+      <c r="Q25" s="22">
         <f t="array" ref="Q25">INDEX($F$2:$G$91,MATCH($K25&amp;Q$1&amp;$I25,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.04074000000003</v>
       </c>
-      <c r="R25" s="7" cm="1">
+      <c r="R25" s="6">
         <f t="array" ref="R25">INDEX($F$2:$G$91,MATCH($K25&amp;R$1&amp;$I25,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>1.01E-3</v>
       </c>
@@ -4208,35 +4191,35 @@
       <c r="I26" s="4">
         <v>50</v>
       </c>
-      <c r="J26" s="27"/>
+      <c r="J26" s="25"/>
       <c r="K26" s="19">
         <v>6</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="M26" s="6" cm="1">
+      <c r="M26" s="22">
         <f t="array" ref="M26">INDEX($F$2:$G$91,MATCH($K26&amp;M$1&amp;$I26,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01089999999999</v>
       </c>
-      <c r="N26" s="7" cm="1">
+      <c r="N26" s="6">
         <f t="array" ref="N26">INDEX($F$2:$G$91,MATCH($K26&amp;N$1&amp;$I26,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.33960000000000001</v>
       </c>
-      <c r="O26" s="6" cm="1">
+      <c r="O26" s="22">
         <f t="array" ref="O26">INDEX($F$2:$G$91,MATCH($K26&amp;O$1&amp;$I26,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01573999999999</v>
       </c>
-      <c r="P26" s="7" cm="1">
+      <c r="P26" s="6">
         <f t="array" ref="P26">INDEX($F$2:$G$91,MATCH($K26&amp;P$1&amp;$I26,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.25947999999999999</v>
       </c>
-      <c r="Q26" s="6" cm="1">
+      <c r="Q26" s="22">
         <f t="array" ref="Q26">INDEX($F$2:$G$91,MATCH($K26&amp;Q$1&amp;$I26,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.02186</v>
       </c>
-      <c r="R26" s="7" cm="1">
+      <c r="R26" s="6">
         <f t="array" ref="R26">INDEX($F$2:$G$91,MATCH($K26&amp;R$1&amp;$I26,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>1.6250000000000001E-2</v>
       </c>
@@ -4266,35 +4249,35 @@
       <c r="I27" s="4">
         <v>50</v>
       </c>
-      <c r="J27" s="28"/>
+      <c r="J27" s="26"/>
       <c r="K27" s="20">
         <v>7</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="11">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M27" s="10" cm="1">
+      <c r="M27" s="23">
         <f t="array" ref="M27">INDEX($F$2:$G$91,MATCH($K27&amp;M$1&amp;$I27,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01513</v>
       </c>
-      <c r="N27" s="11" cm="1">
+      <c r="N27" s="8">
         <f t="array" ref="N27">INDEX($F$2:$G$91,MATCH($K27&amp;N$1&amp;$I27,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.40153</v>
       </c>
-      <c r="O27" s="10" cm="1">
+      <c r="O27" s="23">
         <f t="array" ref="O27">INDEX($F$2:$G$91,MATCH($K27&amp;O$1&amp;$I27,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.02773000000002</v>
       </c>
-      <c r="P27" s="11" cm="1">
+      <c r="P27" s="8">
         <f t="array" ref="P27">INDEX($F$2:$G$91,MATCH($K27&amp;P$1&amp;$I27,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.30647999999999997</v>
       </c>
-      <c r="Q27" s="10" cm="1">
+      <c r="Q27" s="23">
         <f t="array" ref="Q27">INDEX($F$2:$G$91,MATCH($K27&amp;Q$1&amp;$I27,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.02686</v>
       </c>
-      <c r="R27" s="11" cm="1">
+      <c r="R27" s="8">
         <f t="array" ref="R27">INDEX($F$2:$G$91,MATCH($K27&amp;R$1&amp;$I27,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>7.8380000000000005E-2</v>
       </c>
@@ -4324,37 +4307,37 @@
       <c r="I28" s="4">
         <v>60</v>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="24">
         <v>60</v>
       </c>
       <c r="K28" s="18">
         <v>2</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M28" s="8" cm="1">
+      <c r="M28" s="21">
         <f t="array" ref="M28">INDEX($F$2:$G$91,MATCH($K28&amp;M$1&amp;$I28,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>7.0299999999999998E-3</v>
       </c>
-      <c r="N28" s="9" cm="1">
+      <c r="N28" s="7">
         <f t="array" ref="N28">INDEX($F$2:$G$91,MATCH($K28&amp;N$1&amp;$I28,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="O28" s="8" cm="1">
+      <c r="O28" s="21">
         <f t="array" ref="O28">INDEX($F$2:$G$91,MATCH($K28&amp;O$1&amp;$I28,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>7.0800000000000004E-3</v>
       </c>
-      <c r="P28" s="9" cm="1">
+      <c r="P28" s="7">
         <f t="array" ref="P28">INDEX($F$2:$G$91,MATCH($K28&amp;P$1&amp;$I28,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="8" cm="1">
+      <c r="Q28" s="21">
         <f t="array" ref="Q28">INDEX($F$2:$G$91,MATCH($K28&amp;Q$1&amp;$I28,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>1.1809999999999999E-2</v>
       </c>
-      <c r="R28" s="9" cm="1">
+      <c r="R28" s="7">
         <f t="array" ref="R28">INDEX($F$2:$G$91,MATCH($K28&amp;R$1&amp;$I28,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -4384,35 +4367,35 @@
       <c r="I29" s="4">
         <v>60</v>
       </c>
-      <c r="J29" s="27"/>
+      <c r="J29" s="25"/>
       <c r="K29" s="19">
         <v>3</v>
       </c>
-      <c r="L29" s="13">
+      <c r="L29" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M29" s="6" cm="1">
+      <c r="M29" s="22">
         <f t="array" ref="M29">INDEX($F$2:$G$91,MATCH($K29&amp;M$1&amp;$I29,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00855000000001</v>
       </c>
-      <c r="N29" s="7" cm="1">
+      <c r="N29" s="6">
         <f t="array" ref="N29">INDEX($F$2:$G$91,MATCH($K29&amp;N$1&amp;$I29,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>2.4709999999999999E-2</v>
       </c>
-      <c r="O29" s="6" cm="1">
+      <c r="O29" s="22">
         <f t="array" ref="O29">INDEX($F$2:$G$91,MATCH($K29&amp;O$1&amp;$I29,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>7.8380000000000005E-2</v>
       </c>
-      <c r="P29" s="7" cm="1">
+      <c r="P29" s="6">
         <f t="array" ref="P29">INDEX($F$2:$G$91,MATCH($K29&amp;P$1&amp;$I29,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q29" s="6" cm="1">
+      <c r="Q29" s="22">
         <f t="array" ref="Q29">INDEX($F$2:$G$91,MATCH($K29&amp;Q$1&amp;$I29,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>3.2820000000000002E-2</v>
       </c>
-      <c r="R29" s="7" cm="1">
+      <c r="R29" s="6">
         <f t="array" ref="R29">INDEX($F$2:$G$91,MATCH($K29&amp;R$1&amp;$I29,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -4442,35 +4425,35 @@
       <c r="I30" s="4">
         <v>60</v>
       </c>
-      <c r="J30" s="27"/>
+      <c r="J30" s="25"/>
       <c r="K30" s="19">
         <v>4</v>
       </c>
-      <c r="L30" s="13">
+      <c r="L30" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M30" s="6" cm="1">
+      <c r="M30" s="22">
         <f t="array" ref="M30">INDEX($F$2:$G$91,MATCH($K30&amp;M$1&amp;$I30,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.01168000000001</v>
       </c>
-      <c r="N30" s="7" cm="1">
+      <c r="N30" s="6">
         <f t="array" ref="N30">INDEX($F$2:$G$91,MATCH($K30&amp;N$1&amp;$I30,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.10256</v>
       </c>
-      <c r="O30" s="6" cm="1">
+      <c r="O30" s="22">
         <f t="array" ref="O30">INDEX($F$2:$G$91,MATCH($K30&amp;O$1&amp;$I30,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01184999999998</v>
       </c>
-      <c r="P30" s="7" cm="1">
+      <c r="P30" s="6">
         <f t="array" ref="P30">INDEX($F$2:$G$91,MATCH($K30&amp;P$1&amp;$I30,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>2.8729999999999999E-2</v>
       </c>
-      <c r="Q30" s="6" cm="1">
+      <c r="Q30" s="22">
         <f t="array" ref="Q30">INDEX($F$2:$G$91,MATCH($K30&amp;Q$1&amp;$I30,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>0.15618000000000001</v>
       </c>
-      <c r="R30" s="7" cm="1">
+      <c r="R30" s="6">
         <f t="array" ref="R30">INDEX($F$2:$G$91,MATCH($K30&amp;R$1&amp;$I30,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>0</v>
       </c>
@@ -4500,35 +4483,35 @@
       <c r="I31" s="4">
         <v>60</v>
       </c>
-      <c r="J31" s="27"/>
+      <c r="J31" s="25"/>
       <c r="K31" s="19">
         <v>5</v>
       </c>
-      <c r="L31" s="13">
+      <c r="L31" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="M31" s="6" cm="1">
+      <c r="M31" s="22">
         <f t="array" ref="M31">INDEX($F$2:$G$91,MATCH($K31&amp;M$1&amp;$I31,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00841000000003</v>
       </c>
-      <c r="N31" s="7" cm="1">
+      <c r="N31" s="6">
         <f t="array" ref="N31">INDEX($F$2:$G$91,MATCH($K31&amp;N$1&amp;$I31,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.23433000000000001</v>
       </c>
-      <c r="O31" s="6" cm="1">
+      <c r="O31" s="22">
         <f t="array" ref="O31">INDEX($F$2:$G$91,MATCH($K31&amp;O$1&amp;$I31,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01488000000001</v>
       </c>
-      <c r="P31" s="7" cm="1">
+      <c r="P31" s="6">
         <f t="array" ref="P31">INDEX($F$2:$G$91,MATCH($K31&amp;P$1&amp;$I31,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.12731000000000001</v>
       </c>
-      <c r="Q31" s="6" cm="1">
+      <c r="Q31" s="22">
         <f t="array" ref="Q31">INDEX($F$2:$G$91,MATCH($K31&amp;Q$1&amp;$I31,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.01792999999998</v>
       </c>
-      <c r="R31" s="7" cm="1">
+      <c r="R31" s="6">
         <f t="array" ref="R31">INDEX($F$2:$G$91,MATCH($K31&amp;R$1&amp;$I31,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>1.01E-3</v>
       </c>
@@ -4558,35 +4541,35 @@
       <c r="I32" s="4">
         <v>60</v>
       </c>
-      <c r="J32" s="27"/>
+      <c r="J32" s="25"/>
       <c r="K32" s="19">
         <v>6</v>
       </c>
-      <c r="L32" s="13">
+      <c r="L32" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="M32" s="6" cm="1">
+      <c r="M32" s="22">
         <f t="array" ref="M32">INDEX($F$2:$G$91,MATCH($K32&amp;M$1&amp;$I32,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.00977</v>
       </c>
-      <c r="N32" s="7" cm="1">
+      <c r="N32" s="6">
         <f t="array" ref="N32">INDEX($F$2:$G$91,MATCH($K32&amp;N$1&amp;$I32,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.33960000000000001</v>
       </c>
-      <c r="O32" s="6" cm="1">
+      <c r="O32" s="22">
         <f t="array" ref="O32">INDEX($F$2:$G$91,MATCH($K32&amp;O$1&amp;$I32,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.01537999999999</v>
       </c>
-      <c r="P32" s="7" cm="1">
+      <c r="P32" s="6">
         <f t="array" ref="P32">INDEX($F$2:$G$91,MATCH($K32&amp;P$1&amp;$I32,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.25947999999999999</v>
       </c>
-      <c r="Q32" s="6" cm="1">
+      <c r="Q32" s="22">
         <f t="array" ref="Q32">INDEX($F$2:$G$91,MATCH($K32&amp;Q$1&amp;$I32,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.02845000000002</v>
       </c>
-      <c r="R32" s="7" cm="1">
+      <c r="R32" s="6">
         <f t="array" ref="R32">INDEX($F$2:$G$91,MATCH($K32&amp;R$1&amp;$I32,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>1.6250000000000001E-2</v>
       </c>
@@ -4616,35 +4599,35 @@
       <c r="I33" s="4">
         <v>60</v>
       </c>
-      <c r="J33" s="28"/>
+      <c r="J33" s="26"/>
       <c r="K33" s="20">
         <v>7</v>
       </c>
-      <c r="L33" s="14">
+      <c r="L33" s="11">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M33" s="10" cm="1">
+      <c r="M33" s="23">
         <f t="array" ref="M33">INDEX($F$2:$G$91,MATCH($K33&amp;M$1&amp;$I33,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(M$3,$F$1:$G$1,0))</f>
         <v>300.02132999999998</v>
       </c>
-      <c r="N33" s="11" cm="1">
+      <c r="N33" s="8">
         <f t="array" ref="N33">INDEX($F$2:$G$91,MATCH($K33&amp;N$1&amp;$I33,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(N$3,$F$1:$G$1,0))</f>
         <v>0.40153</v>
       </c>
-      <c r="O33" s="10" cm="1">
+      <c r="O33" s="23">
         <f t="array" ref="O33">INDEX($F$2:$G$91,MATCH($K33&amp;O$1&amp;$I33,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(O$3,$F$1:$G$1,0))</f>
         <v>300.03303</v>
       </c>
-      <c r="P33" s="11" cm="1">
+      <c r="P33" s="8">
         <f t="array" ref="P33">INDEX($F$2:$G$91,MATCH($K33&amp;P$1&amp;$I33,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(P$3,$F$1:$G$1,0))</f>
         <v>0.30647999999999997</v>
       </c>
-      <c r="Q33" s="10" cm="1">
+      <c r="Q33" s="23">
         <f t="array" ref="Q33">INDEX($F$2:$G$91,MATCH($K33&amp;Q$1&amp;$I33,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(Q$3,$F$1:$G$1,0))</f>
         <v>300.02677999999997</v>
       </c>
-      <c r="R33" s="11" cm="1">
+      <c r="R33" s="8">
         <f t="array" ref="R33">INDEX($F$2:$G$91,MATCH($K33&amp;R$1&amp;$I33,$C$2:$C$91&amp;$D$2:$D$91&amp;$E$2:$E$91,0),MATCH(R$3,$F$1:$G$1,0))</f>
         <v>7.8380000000000005E-2</v>
       </c>
@@ -6048,7 +6031,7 @@
       <c r="J93" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G91" xr:uid="{3F336A05-40B4-2F49-8B4D-534C0624117E}">
+  <autoFilter ref="A1:G91" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G91">
       <sortCondition ref="E1:E91"/>
     </sortState>

</xml_diff>

<commit_message>
fixed bug in visit percentage and bug in create instances
</commit_message>
<xml_diff>
--- a/computational_study/comp_study_summary.xlsx
+++ b/computational_study/comp_study_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tordhaflan/Dropbox/NTNU/Master/master-thesis/computational_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D56D2A-F11C-CF40-85B2-F780DF73EC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891561D9-870E-6249-A64E-0E19DB7097CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2739,7 +2739,7 @@
   <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="126" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added feature to run same data on alternative/standard in same instance with same parameters
</commit_message>
<xml_diff>
--- a/computational_study/comp_study_summary.xlsx
+++ b/computational_study/comp_study_summary.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Comp study" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="CS Test" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="19-11 03.27" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="23-11 15.13" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="23-11 15.39" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'CS Test'!$A$1:$G$91</definedName>
@@ -7175,19 +7175,19 @@
         <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>10.00896</v>
+        <v>60.03342</v>
       </c>
       <c r="G2" t="n">
-        <v>0.19635</v>
+        <v>0.14804</v>
       </c>
       <c r="H2" t="n">
-        <v>0.10526</v>
+        <v>0.18421</v>
       </c>
       <c r="I2" t="n">
         <v>6.70045</v>
@@ -7209,22 +7209,22 @@
         <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>10.00608</v>
+        <v>60.0083</v>
       </c>
       <c r="G3" t="n">
-        <v>0.16404</v>
+        <v>0.24404</v>
       </c>
       <c r="H3" t="n">
-        <v>0.33333</v>
+        <v>0.47368</v>
       </c>
       <c r="I3" t="n">
-        <v>7.62</v>
+        <v>7.13</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
implemented subtour elimination of sets of length 2 and 3
</commit_message>
<xml_diff>
--- a/computational_study/comp_study_summary.xlsx
+++ b/computational_study/comp_study_summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="20540" windowWidth="33600" xWindow="0" yWindow="460"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="23540" windowWidth="38400" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="Comp study" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,10 @@
     <sheet name="24-11 03.28" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="24-11 12.20" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="24-11 12.21" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="24-11 18.12" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="24-11 18.52" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="24-11 18.53" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="24-11 18.54" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'CS Test'!$A$1:$G$91</definedName>
@@ -30,7 +34,7 @@
     <numFmt formatCode="0.0%" numFmtId="165"/>
     <numFmt formatCode="\V\ \=\ #,##0" numFmtId="166"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -88,6 +92,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -99,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -274,6 +283,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -285,7 +320,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -345,6 +380,9 @@
     <xf applyAlignment="1" borderId="14" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf applyAlignment="1" borderId="15" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf applyAlignment="1" borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,7 +391,10 @@
     <xf applyAlignment="1" borderId="10" fillId="0" fontId="4" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2852,6 +2893,238 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="35" t="inlineStr">
+        <is>
+          <t>Zones</t>
+        </is>
+      </c>
+      <c r="C1" s="35" t="inlineStr">
+        <is>
+          <t>Nodes per zone</t>
+        </is>
+      </c>
+      <c r="D1" s="35" t="inlineStr">
+        <is>
+          <t>Number of vehicles</t>
+        </is>
+      </c>
+      <c r="E1" s="35" t="inlineStr">
+        <is>
+          <t>T_max</t>
+        </is>
+      </c>
+      <c r="F1" s="35" t="inlineStr">
+        <is>
+          <t>Solution time</t>
+        </is>
+      </c>
+      <c r="G1" s="35" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="H1" s="35" t="inlineStr">
+        <is>
+          <t>Visit percent</t>
+        </is>
+      </c>
+      <c r="I1" s="35" t="inlineStr">
+        <is>
+          <t>Deviation before</t>
+        </is>
+      </c>
+      <c r="J1" s="35" t="inlineStr">
+        <is>
+          <t>Deviation after</t>
+        </is>
+      </c>
+      <c r="K1" s="35" t="inlineStr">
+        <is>
+          <t>Obj value</t>
+        </is>
+      </c>
+      <c r="L1" s="35" t="inlineStr">
+        <is>
+          <t>Model type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10.01034</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.45652</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.78571</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="35" t="inlineStr">
+        <is>
+          <t>Zones</t>
+        </is>
+      </c>
+      <c r="C1" s="35" t="inlineStr">
+        <is>
+          <t>Nodes per zone</t>
+        </is>
+      </c>
+      <c r="D1" s="35" t="inlineStr">
+        <is>
+          <t>Number of vehicles</t>
+        </is>
+      </c>
+      <c r="E1" s="35" t="inlineStr">
+        <is>
+          <t>T_max</t>
+        </is>
+      </c>
+      <c r="F1" s="35" t="inlineStr">
+        <is>
+          <t>Solution time</t>
+        </is>
+      </c>
+      <c r="G1" s="35" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="H1" s="35" t="inlineStr">
+        <is>
+          <t>Visit percent</t>
+        </is>
+      </c>
+      <c r="I1" s="35" t="inlineStr">
+        <is>
+          <t>Deviation before</t>
+        </is>
+      </c>
+      <c r="J1" s="35" t="inlineStr">
+        <is>
+          <t>Deviation after</t>
+        </is>
+      </c>
+      <c r="K1" s="35" t="inlineStr">
+        <is>
+          <t>Obj value</t>
+        </is>
+      </c>
+      <c r="L1" s="35" t="inlineStr">
+        <is>
+          <t>Model type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2" t="n">
+        <v>60.00966</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.09903000000000001</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.78571</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -2860,8 +3133,8 @@
   </sheetPr>
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0" zoomScale="126">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0" zoomScale="126">
+      <selection activeCell="L7" sqref="L7:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2953,18 +3226,18 @@
       </c>
       <c r="K2" s="12" t="n"/>
       <c r="L2" s="12" t="n"/>
-      <c r="M2" s="32" t="n">
+      <c r="M2" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="31" t="n"/>
-      <c r="O2" s="32" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" s="31" t="n"/>
-      <c r="Q2" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="R2" s="31" t="n"/>
+      <c r="N2" s="32" t="n"/>
+      <c r="O2" s="33" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" s="32" t="n"/>
+      <c r="Q2" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" s="32" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -3059,7 +3332,7 @@
       <c r="I4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="J4" s="29" t="n">
+      <c r="J4" s="30" t="n">
         <v>20</v>
       </c>
       <c r="K4" s="18" t="n">
@@ -3119,7 +3392,7 @@
       <c r="I5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="J5" s="30" t="n"/>
+      <c r="J5" s="31" t="n"/>
       <c r="K5" s="19" t="n">
         <v>3</v>
       </c>
@@ -3177,7 +3450,7 @@
       <c r="I6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="J6" s="30" t="n"/>
+      <c r="J6" s="31" t="n"/>
       <c r="K6" s="19" t="n">
         <v>4</v>
       </c>
@@ -3235,7 +3508,7 @@
       <c r="I7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="J7" s="30" t="n"/>
+      <c r="J7" s="31" t="n"/>
       <c r="K7" s="19" t="n">
         <v>5</v>
       </c>
@@ -3293,7 +3566,7 @@
       <c r="I8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="J8" s="30" t="n"/>
+      <c r="J8" s="31" t="n"/>
       <c r="K8" s="19" t="n">
         <v>6</v>
       </c>
@@ -3351,7 +3624,7 @@
       <c r="I9" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="J9" s="31" t="n"/>
+      <c r="J9" s="32" t="n"/>
       <c r="K9" s="20" t="n">
         <v>7</v>
       </c>
@@ -3409,7 +3682,7 @@
       <c r="I10" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J10" s="29" t="n">
+      <c r="J10" s="30" t="n">
         <v>30</v>
       </c>
       <c r="K10" s="18" t="n">
@@ -3469,7 +3742,7 @@
       <c r="I11" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J11" s="30" t="n"/>
+      <c r="J11" s="31" t="n"/>
       <c r="K11" s="19" t="n">
         <v>3</v>
       </c>
@@ -3527,7 +3800,7 @@
       <c r="I12" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J12" s="30" t="n"/>
+      <c r="J12" s="31" t="n"/>
       <c r="K12" s="19" t="n">
         <v>4</v>
       </c>
@@ -3585,7 +3858,7 @@
       <c r="I13" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J13" s="30" t="n"/>
+      <c r="J13" s="31" t="n"/>
       <c r="K13" s="19" t="n">
         <v>5</v>
       </c>
@@ -3643,7 +3916,7 @@
       <c r="I14" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J14" s="30" t="n"/>
+      <c r="J14" s="31" t="n"/>
       <c r="K14" s="19" t="n">
         <v>6</v>
       </c>
@@ -3701,7 +3974,7 @@
       <c r="I15" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J15" s="31" t="n"/>
+      <c r="J15" s="32" t="n"/>
       <c r="K15" s="20" t="n">
         <v>7</v>
       </c>
@@ -3759,7 +4032,7 @@
       <c r="I16" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="J16" s="29" t="n">
+      <c r="J16" s="30" t="n">
         <v>40</v>
       </c>
       <c r="K16" s="18" t="n">
@@ -3819,7 +4092,7 @@
       <c r="I17" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="J17" s="30" t="n"/>
+      <c r="J17" s="31" t="n"/>
       <c r="K17" s="19" t="n">
         <v>3</v>
       </c>
@@ -3877,7 +4150,7 @@
       <c r="I18" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="J18" s="30" t="n"/>
+      <c r="J18" s="31" t="n"/>
       <c r="K18" s="19" t="n">
         <v>4</v>
       </c>
@@ -3935,7 +4208,7 @@
       <c r="I19" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="J19" s="30" t="n"/>
+      <c r="J19" s="31" t="n"/>
       <c r="K19" s="19" t="n">
         <v>5</v>
       </c>
@@ -3993,7 +4266,7 @@
       <c r="I20" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="J20" s="30" t="n"/>
+      <c r="J20" s="31" t="n"/>
       <c r="K20" s="19" t="n">
         <v>6</v>
       </c>
@@ -4051,7 +4324,7 @@
       <c r="I21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="J21" s="31" t="n"/>
+      <c r="J21" s="32" t="n"/>
       <c r="K21" s="20" t="n">
         <v>7</v>
       </c>
@@ -4109,7 +4382,7 @@
       <c r="I22" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J22" s="29" t="n">
+      <c r="J22" s="30" t="n">
         <v>50</v>
       </c>
       <c r="K22" s="18" t="n">
@@ -4169,7 +4442,7 @@
       <c r="I23" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J23" s="30" t="n"/>
+      <c r="J23" s="31" t="n"/>
       <c r="K23" s="19" t="n">
         <v>3</v>
       </c>
@@ -4227,7 +4500,7 @@
       <c r="I24" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J24" s="30" t="n"/>
+      <c r="J24" s="31" t="n"/>
       <c r="K24" s="19" t="n">
         <v>4</v>
       </c>
@@ -4285,7 +4558,7 @@
       <c r="I25" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J25" s="30" t="n"/>
+      <c r="J25" s="31" t="n"/>
       <c r="K25" s="19" t="n">
         <v>5</v>
       </c>
@@ -4343,7 +4616,7 @@
       <c r="I26" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J26" s="30" t="n"/>
+      <c r="J26" s="31" t="n"/>
       <c r="K26" s="19" t="n">
         <v>6</v>
       </c>
@@ -4401,7 +4674,7 @@
       <c r="I27" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J27" s="31" t="n"/>
+      <c r="J27" s="32" t="n"/>
       <c r="K27" s="20" t="n">
         <v>7</v>
       </c>
@@ -4459,7 +4732,7 @@
       <c r="I28" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="J28" s="29" t="n">
+      <c r="J28" s="30" t="n">
         <v>60</v>
       </c>
       <c r="K28" s="18" t="n">
@@ -4519,7 +4792,7 @@
       <c r="I29" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="J29" s="30" t="n"/>
+      <c r="J29" s="31" t="n"/>
       <c r="K29" s="19" t="n">
         <v>3</v>
       </c>
@@ -4577,7 +4850,7 @@
       <c r="I30" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="J30" s="30" t="n"/>
+      <c r="J30" s="31" t="n"/>
       <c r="K30" s="19" t="n">
         <v>4</v>
       </c>
@@ -4635,7 +4908,7 @@
       <c r="I31" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="J31" s="30" t="n"/>
+      <c r="J31" s="31" t="n"/>
       <c r="K31" s="19" t="n">
         <v>5</v>
       </c>
@@ -4693,7 +4966,7 @@
       <c r="I32" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="J32" s="30" t="n"/>
+      <c r="J32" s="31" t="n"/>
       <c r="K32" s="19" t="n">
         <v>6</v>
       </c>
@@ -4751,7 +5024,7 @@
       <c r="I33" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="J33" s="31" t="n"/>
+      <c r="J33" s="32" t="n"/>
       <c r="K33" s="20" t="n">
         <v>7</v>
       </c>
@@ -7735,7 +8008,7 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:L2"/>
     </sheetView>
   </sheetViews>
@@ -7909,67 +8182,67 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="33" t="inlineStr">
+      <c r="B1" s="29" t="inlineStr">
         <is>
           <t>Zones</t>
         </is>
       </c>
-      <c r="C1" s="33" t="inlineStr">
+      <c r="C1" s="29" t="inlineStr">
         <is>
           <t>Nodes per zone</t>
         </is>
       </c>
-      <c r="D1" s="33" t="inlineStr">
+      <c r="D1" s="29" t="inlineStr">
         <is>
           <t>Number of vehicles</t>
         </is>
       </c>
-      <c r="E1" s="33" t="inlineStr">
+      <c r="E1" s="29" t="inlineStr">
         <is>
           <t>T_max</t>
         </is>
       </c>
-      <c r="F1" s="33" t="inlineStr">
+      <c r="F1" s="29" t="inlineStr">
         <is>
           <t>Solution time</t>
         </is>
       </c>
-      <c r="G1" s="33" t="inlineStr">
+      <c r="G1" s="29" t="inlineStr">
         <is>
           <t>Gap</t>
         </is>
       </c>
-      <c r="H1" s="33" t="inlineStr">
+      <c r="H1" s="29" t="inlineStr">
         <is>
           <t>Visit percent</t>
         </is>
       </c>
-      <c r="I1" s="33" t="inlineStr">
+      <c r="I1" s="29" t="inlineStr">
         <is>
           <t>Deviation before</t>
         </is>
       </c>
-      <c r="J1" s="33" t="inlineStr">
+      <c r="J1" s="29" t="inlineStr">
         <is>
           <t>Deviation after</t>
         </is>
       </c>
-      <c r="K1" s="33" t="inlineStr">
+      <c r="K1" s="29" t="inlineStr">
         <is>
           <t>Obj value</t>
         </is>
       </c>
-      <c r="L1" s="33" t="inlineStr">
+      <c r="L1" s="29" t="inlineStr">
         <is>
           <t>Model type</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="33" t="n">
+      <c r="A2" s="29" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -8009,7 +8282,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="n">
+      <c r="A3" s="29" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -8049,7 +8322,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="33" t="n">
+      <c r="A4" s="29" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
@@ -8089,7 +8362,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="33" t="n">
+      <c r="A5" s="29" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
@@ -8129,7 +8402,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="33" t="n">
+      <c r="A6" s="29" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
@@ -8169,7 +8442,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="n">
+      <c r="A7" s="29" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
@@ -8209,7 +8482,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="33" t="n">
+      <c r="A8" s="29" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
@@ -8249,7 +8522,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="33" t="n">
+      <c r="A9" s="29" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
@@ -8289,7 +8562,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="33" t="n">
+      <c r="A10" s="29" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
@@ -8329,7 +8602,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="n">
+      <c r="A11" s="29" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
@@ -8369,7 +8642,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="n">
+      <c r="A12" s="29" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
@@ -8409,7 +8682,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="n">
+      <c r="A13" s="29" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
@@ -8449,7 +8722,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="n">
+      <c r="A14" s="29" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
@@ -8494,6 +8767,621 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="226">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="5" width="3.1640625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="5" width="5.6640625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="5" width="13"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="5" width="16"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="5" width="6"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="5" width="11.6640625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="5" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="5" width="11.1640625"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="5" width="14.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="5" width="12.6640625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="5" width="9.1640625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="5" width="10.1640625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="29" t="inlineStr">
+        <is>
+          <t>Zones</t>
+        </is>
+      </c>
+      <c r="C1" s="29" t="inlineStr">
+        <is>
+          <t>Nodes per zone</t>
+        </is>
+      </c>
+      <c r="D1" s="29" t="inlineStr">
+        <is>
+          <t>Number of vehicles</t>
+        </is>
+      </c>
+      <c r="E1" s="29" t="inlineStr">
+        <is>
+          <t>T_max</t>
+        </is>
+      </c>
+      <c r="F1" s="29" t="inlineStr">
+        <is>
+          <t>Solution time</t>
+        </is>
+      </c>
+      <c r="G1" s="29" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="H1" s="29" t="inlineStr">
+        <is>
+          <t>Visit percent</t>
+        </is>
+      </c>
+      <c r="I1" s="29" t="inlineStr">
+        <is>
+          <t>Deviation before</t>
+        </is>
+      </c>
+      <c r="J1" s="29" t="inlineStr">
+        <is>
+          <t>Deviation after</t>
+        </is>
+      </c>
+      <c r="K1" s="29" t="inlineStr">
+        <is>
+          <t>Obj value</t>
+        </is>
+      </c>
+      <c r="L1" s="29" t="inlineStr">
+        <is>
+          <t>Model type</t>
+        </is>
+      </c>
+      <c r="M1" s="34" t="inlineStr">
+        <is>
+          <t>Standard objective</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>30.017</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.32297</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22</v>
+      </c>
+      <c r="F3" t="n">
+        <v>120.04342</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.26703</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>26</v>
+      </c>
+      <c r="F4" t="n">
+        <v>11.9072</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K4" t="n">
+        <v>9.5175</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>120.01372</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.27394</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>26</v>
+      </c>
+      <c r="F6" t="n">
+        <v>120.01564</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.21851</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I6" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="K6" t="n">
+        <v>8.970000000000001</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.80117</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.66667</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7.50286</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>22</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.17971</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="K8" t="n">
+        <v>6.70667</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="29" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.38462</v>
+      </c>
+      <c r="I9" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="29" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>14.72569</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.57692</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10.77036</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="29" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.92159</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.72727</v>
+      </c>
+      <c r="I11" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="K11" t="n">
+        <v>11.976</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="29" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>120.01614</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.37514</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.88462</v>
+      </c>
+      <c r="I12" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K12" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F13" t="n">
+        <v>120.02723</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.37201</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.95455</v>
+      </c>
+      <c r="I13" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>8.789999999999999</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="29" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>18</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.13596</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.76923</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8508,95 +9396,691 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="33" t="inlineStr">
+      <c r="B1" s="35" t="inlineStr">
         <is>
           <t>Zones</t>
         </is>
       </c>
-      <c r="C1" s="33" t="inlineStr">
+      <c r="C1" s="35" t="inlineStr">
         <is>
           <t>Nodes per zone</t>
         </is>
       </c>
-      <c r="D1" s="33" t="inlineStr">
+      <c r="D1" s="35" t="inlineStr">
         <is>
           <t>Number of vehicles</t>
         </is>
       </c>
-      <c r="E1" s="33" t="inlineStr">
+      <c r="E1" s="35" t="inlineStr">
         <is>
           <t>T_max</t>
         </is>
       </c>
-      <c r="F1" s="33" t="inlineStr">
+      <c r="F1" s="35" t="inlineStr">
         <is>
           <t>Solution time</t>
         </is>
       </c>
-      <c r="G1" s="33" t="inlineStr">
+      <c r="G1" s="35" t="inlineStr">
         <is>
           <t>Gap</t>
         </is>
       </c>
-      <c r="H1" s="33" t="inlineStr">
+      <c r="H1" s="35" t="inlineStr">
         <is>
           <t>Visit percent</t>
         </is>
       </c>
-      <c r="I1" s="33" t="inlineStr">
+      <c r="I1" s="35" t="inlineStr">
         <is>
           <t>Deviation before</t>
         </is>
       </c>
-      <c r="J1" s="33" t="inlineStr">
+      <c r="J1" s="35" t="inlineStr">
         <is>
           <t>Deviation after</t>
         </is>
       </c>
-      <c r="K1" s="33" t="inlineStr">
+      <c r="K1" s="35" t="inlineStr">
         <is>
           <t>Obj value</t>
         </is>
       </c>
-      <c r="L1" s="33" t="inlineStr">
+      <c r="L1" s="35" t="inlineStr">
         <is>
           <t>Model type</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="33" t="n">
+      <c r="A2" s="35" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
       </c>
       <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10.00735</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.11336</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.71429</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22</v>
+      </c>
+      <c r="F3" t="n">
+        <v>120.04342</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.26703</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
         <v>4</v>
       </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>26</v>
+      </c>
+      <c r="F4" t="n">
+        <v>11.9072</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K4" t="n">
+        <v>9.5175</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>120.01372</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.27394</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>26</v>
+      </c>
+      <c r="F6" t="n">
+        <v>120.01564</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.21851</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I6" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="K6" t="n">
+        <v>8.970000000000001</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="35" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.80117</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.66667</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7.50286</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="35" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>22</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.17971</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="K8" t="n">
+        <v>6.70667</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="35" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.38462</v>
+      </c>
+      <c r="I9" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="35" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>14.72569</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.57692</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10.77036</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="35" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.92159</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.72727</v>
+      </c>
+      <c r="I11" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="K11" t="n">
+        <v>11.976</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="35" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>120.01614</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.37514</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.88462</v>
+      </c>
+      <c r="I12" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K12" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="35" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F13" t="n">
+        <v>120.02723</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.37201</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.95455</v>
+      </c>
+      <c r="I13" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>8.789999999999999</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="35" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>18</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.13596</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.76923</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="35" t="inlineStr">
+        <is>
+          <t>Zones</t>
+        </is>
+      </c>
+      <c r="C1" s="35" t="inlineStr">
+        <is>
+          <t>Nodes per zone</t>
+        </is>
+      </c>
+      <c r="D1" s="35" t="inlineStr">
+        <is>
+          <t>Number of vehicles</t>
+        </is>
+      </c>
+      <c r="E1" s="35" t="inlineStr">
+        <is>
+          <t>T_max</t>
+        </is>
+      </c>
+      <c r="F1" s="35" t="inlineStr">
+        <is>
+          <t>Solution time</t>
+        </is>
+      </c>
+      <c r="G1" s="35" t="inlineStr">
+        <is>
+          <t>Gap</t>
+        </is>
+      </c>
+      <c r="H1" s="35" t="inlineStr">
+        <is>
+          <t>Visit percent</t>
+        </is>
+      </c>
+      <c r="I1" s="35" t="inlineStr">
+        <is>
+          <t>Deviation before</t>
+        </is>
+      </c>
+      <c r="J1" s="35" t="inlineStr">
+        <is>
+          <t>Deviation after</t>
+        </is>
+      </c>
+      <c r="K1" s="35" t="inlineStr">
+        <is>
+          <t>Obj value</t>
+        </is>
+      </c>
+      <c r="L1" s="35" t="inlineStr">
+        <is>
+          <t>Model type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" t="n">
-        <v>30.017</v>
+        <v>120.04342</v>
       </c>
       <c r="G2" t="n">
-        <v>0.32297</v>
+        <v>0.26703</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>8.33</v>
+        <v>6.59</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>7.4</v>
+        <v>5.58</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -8605,447 +10089,447 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="n">
+      <c r="A3" s="35" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
+        <v>26</v>
+      </c>
+      <c r="F3" t="n">
+        <v>11.9072</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>9.5175</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>120.01372</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.27394</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>26</v>
+      </c>
+      <c r="F5" t="n">
+        <v>120.01564</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.21851</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I5" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8.970000000000001</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.80117</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.66667</v>
+      </c>
+      <c r="I6" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="K6" t="n">
+        <v>7.50286</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="35" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
         <v>22</v>
       </c>
-      <c r="F3" t="n">
-        <v>120.04342</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.26703</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="F7" t="n">
+        <v>0.17971</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I7" t="n">
         <v>6.59</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>5.58</v>
-      </c>
-      <c r="L3" t="inlineStr">
+      <c r="J7" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="K7" t="n">
+        <v>6.70667</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="35" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.38462</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="35" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14.72569</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.57692</v>
+      </c>
+      <c r="I9" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="K9" t="n">
+        <v>10.77036</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="35" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12.92159</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.72727</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="K10" t="n">
+        <v>11.976</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="35" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+      <c r="F11" t="n">
+        <v>120.01614</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.37514</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.88462</v>
+      </c>
+      <c r="I11" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K11" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>Standard</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
+    <row r="12">
+      <c r="A12" s="35" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>26</v>
-      </c>
-      <c r="F4" t="n">
-        <v>11.9072</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="I4" t="n">
-        <v>7.71</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="K4" t="n">
-        <v>9.5175</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Alternative</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F5" t="n">
-        <v>120.01372</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.27394</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>7.77</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>8.25</v>
-      </c>
-      <c r="L5" t="inlineStr">
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F12" t="n">
+        <v>120.02723</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.37201</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.95455</v>
+      </c>
+      <c r="I12" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8.789999999999999</v>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>Standard</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="33" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="n">
-        <v>26</v>
-      </c>
-      <c r="F6" t="n">
-        <v>120.01564</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.21851</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="I6" t="n">
-        <v>7.71</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="K6" t="n">
-        <v>8.970000000000001</v>
-      </c>
-      <c r="L6" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="35" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>18</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2.13596</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.76923</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>Standard</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="33" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>25</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.80117</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.66667</v>
-      </c>
-      <c r="I7" t="n">
-        <v>7.77</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.59</v>
-      </c>
-      <c r="K7" t="n">
-        <v>7.50286</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Alternative</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="33" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>22</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.17971</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I8" t="n">
-        <v>6.59</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="K8" t="n">
-        <v>6.70667</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Alternative</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="33" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" t="n">
-        <v>18</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0344</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.38462</v>
-      </c>
-      <c r="I9" t="n">
-        <v>4.41</v>
-      </c>
-      <c r="J9" t="n">
-        <v>2.14</v>
-      </c>
-      <c r="K9" t="n">
-        <v>4.53</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Alternative</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="33" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" t="n">
-        <v>25</v>
-      </c>
-      <c r="F10" t="n">
-        <v>14.72569</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.57692</v>
-      </c>
-      <c r="I10" t="n">
-        <v>9.57</v>
-      </c>
-      <c r="J10" t="n">
-        <v>2.19</v>
-      </c>
-      <c r="K10" t="n">
-        <v>10.77036</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Alternative</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="33" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3</v>
-      </c>
-      <c r="E11" t="n">
-        <v>30</v>
-      </c>
-      <c r="F11" t="n">
-        <v>12.92159</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.72727</v>
-      </c>
-      <c r="I11" t="n">
-        <v>9.48</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="K11" t="n">
-        <v>11.976</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Alternative</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="33" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>25</v>
-      </c>
-      <c r="F12" t="n">
-        <v>120.01614</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.37514</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.88462</v>
-      </c>
-      <c r="I12" t="n">
-        <v>9.57</v>
-      </c>
-      <c r="J12" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="K12" t="n">
-        <v>9.17</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="33" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="n">
-        <v>4</v>
-      </c>
-      <c r="D13" t="n">
-        <v>3</v>
-      </c>
-      <c r="E13" t="n">
-        <v>30</v>
-      </c>
-      <c r="F13" t="n">
-        <v>120.02723</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.37201</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.95455</v>
-      </c>
-      <c r="I13" t="n">
-        <v>9.48</v>
-      </c>
-      <c r="J13" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" t="n">
-        <v>8.789999999999999</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-    </row>
     <row r="14">
-      <c r="A14" s="33" t="n">
+      <c r="A14" s="35" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
@@ -9058,25 +10542,25 @@
         <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F14" t="n">
-        <v>2.13596</v>
+        <v>10.0176</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.45652</v>
       </c>
       <c r="H14" t="n">
-        <v>0.76923</v>
+        <v>0.78571</v>
       </c>
       <c r="I14" t="n">
-        <v>4.41</v>
+        <v>5.66</v>
       </c>
       <c r="J14" t="n">
-        <v>0.32</v>
+        <v>1.8</v>
       </c>
       <c r="K14" t="n">
-        <v>4.5</v>
+        <v>4.14</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>

</xml_diff>